<commit_message>
clientNo and groupNo in excel template
</commit_message>
<xml_diff>
--- a/excel/GstAccount.xlsx
+++ b/excel/GstAccount.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\itportal\portalweb\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\itportal\portal\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4118D370-45B5-44FA-9405-6F20EA16EDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E1D6EC-E753-4918-85B1-1772AB63A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F8D38D3E-3D70-44EA-9D49-3808D87505ED}"/>
+    <workbookView xWindow="7200" yWindow="4095" windowWidth="21600" windowHeight="11385" xr2:uid="{F8D38D3E-3D70-44EA-9D49-3808D87505ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -44,7 +44,10 @@
     <t>portalUserName</t>
   </si>
   <si>
-    <t>client code</t>
+    <t>clientNo</t>
+  </si>
+  <si>
+    <t>groupNo</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A827DD05-D30B-4E82-9F0E-4B8BFF6ECD77}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +423,7 @@
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +436,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
   </sheetData>

</xml_diff>